<commit_message>
Added remove button, updated itext template, added a new form in the testing cache, became less strict about itext retrieval
</commit_message>
<xml_diff>
--- a/templates/itext_template.xlsx
+++ b/templates/itext_template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Language</t>
   </si>
@@ -36,46 +36,24 @@
     <t>Video</t>
   </si>
   <si>
-    <t>question1</t>
-  </si>
-  <si>
-    <t>question2</t>
-  </si>
-  <si>
-    <t>question3</t>
-  </si>
-  <si>
-    <t>en</t>
-  </si>
-  <si>
-    <t>pt</t>
-  </si>
-  <si>
-    <t>So what's your name?</t>
-  </si>
-  <si>
-    <t>Are you male or female?</t>
-  </si>
-  <si>
-    <t>question4</t>
-  </si>
-  <si>
-    <t>some audio</t>
-  </si>
-  <si>
-    <t>jr://image/uri/some.png</t>
-  </si>
-  <si>
-    <t>hahah q3 audio only</t>
+    <t>PASTE HERE!!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -90,7 +68,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -98,12 +76,72 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,110 +436,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="19.5" thickBot="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>